<commit_message>
Fix cell calculation errors in RGB-CMY templates
</commit_message>
<xml_diff>
--- a/data/templates/RGB-CMY Channel analysis.xlsx
+++ b/data/templates/RGB-CMY Channel analysis.xlsx
@@ -720,8 +720,8 @@
   </sheetPr>
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B48" activeCellId="0" sqref="B48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.671875" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -743,7 +743,7 @@
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
         <f aca="true">NOW()</f>
-        <v>45947.6847460825</v>
+        <v>45948.278860815</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1086,12 +1086,16 @@
         <v>#DIV/0!</v>
       </c>
       <c r="D24" s="14" t="n">
-        <f aca="false">SQRT(C16^2+C17^2+C19^2+C21^2)</f>
+        <f aca="false">SQRT(C16^2+C17^2+C18^2+C19^2+C20^2+C21^2)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="14" t="n">
+        <f aca="false">SQRT(F16^2+F17^2+F18^2+F19^2+F20^2+F21^2)</f>
         <v>0</v>
       </c>
       <c r="H24" s="14"/>
       <c r="J24" s="14" t="n">
-        <f aca="false">SQRT(I16^2+I17^2+I19^2+I21^2)</f>
+        <f aca="false">SQRT(I16^2+I17^2+I18^2+I19^2+I20^2+I21^2)</f>
         <v>0</v>
       </c>
       <c r="K24" s="4"/>
@@ -1358,14 +1362,25 @@
         <f aca="false">SQRT(C35^2+H35^2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="D37" s="25"/>
+      <c r="D37" s="14" t="n">
+        <f aca="false">SQRT(C29^2+C30^2+C31^2+C32^2+C33^2+C34^2)</f>
+        <v>0</v>
+      </c>
+      <c r="G37" s="14" t="n">
+        <f aca="false">SQRT(F29^2+F30^2+F31^2+F32^2+F33^2+F34^2)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="14" t="n">
+        <f aca="false">SQRT(I29^2+I30^2+I31^2+I32^2+I33^2+I34^2)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B38" s="27" t="e">
-        <f aca="false">E35-H35</f>
+        <f aca="false">H35-E35</f>
         <v>#DIV/0!</v>
       </c>
       <c r="C38" s="28" t="e">
@@ -1519,7 +1534,7 @@
         <v>17</v>
       </c>
       <c r="B48" s="13" t="n">
-        <f aca="false">H47-G47</f>
+        <f aca="false">SQRT(C16^2+C17^2+C18^2+C19^2+C20^2+C21^2)</f>
         <v>0</v>
       </c>
       <c r="C48" s="5"/>

</xml_diff>